<commit_message>
Update overlapping ROW edge strategy
</commit_message>
<xml_diff>
--- a/XC-comparisons/14E-DAT_comparison.xlsx
+++ b/XC-comparisons/14E-DAT_comparison.xlsx
@@ -1311,7 +1311,7 @@
         <v>-20</v>
       </c>
       <c r="B32">
-        <v>-0.00100000000000122</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1717,7 +1717,7 @@
         <v>-6</v>
       </c>
       <c r="B46">
-        <v>-0.000999999999997669</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2036,7 +2036,7 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>-0.00100000000000122</v>
+        <v>-3.5527136788005e-15</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2442,7 +2442,7 @@
         <v>19</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>0.000999999999997669</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2500,7 +2500,7 @@
         <v>21</v>
       </c>
       <c r="B73">
-        <v>-0.00100000000000122</v>
+        <v>0</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -7253,7 +7253,7 @@
         <v>-20</v>
       </c>
       <c r="B32">
-        <v>30.014</v>
+        <v>30.015</v>
       </c>
       <c r="C32">
         <v>36.641</v>
@@ -7659,7 +7659,7 @@
         <v>-6</v>
       </c>
       <c r="B46">
-        <v>32.191</v>
+        <v>32.192</v>
       </c>
       <c r="C46">
         <v>36.668</v>
@@ -7978,7 +7978,7 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>29.248</v>
+        <v>29.249</v>
       </c>
       <c r="C57">
         <v>30.31</v>
@@ -8384,7 +8384,7 @@
         <v>19</v>
       </c>
       <c r="B71">
-        <v>20.428</v>
+        <v>20.429</v>
       </c>
       <c r="C71">
         <v>20.454</v>
@@ -8442,7 +8442,7 @@
         <v>21</v>
       </c>
       <c r="B73">
-        <v>19.212</v>
+        <v>19.213</v>
       </c>
       <c r="C73">
         <v>19.221</v>
@@ -10224,7 +10224,7 @@
         <v>-20</v>
       </c>
       <c r="B32">
-        <v>-0.00333177850336917</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -10630,7 +10630,7 @@
         <v>-6</v>
       </c>
       <c r="B46">
-        <v>-0.00310645832685431</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -10949,7 +10949,7 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>-0.0034190371991289</v>
+        <v>-1.21464449341875e-14</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -11355,7 +11355,7 @@
         <v>19</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>0.00489500220273958</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -11413,7 +11413,7 @@
         <v>21</v>
       </c>
       <c r="B73">
-        <v>-0.0052050801582408</v>
+        <v>0</v>
       </c>
       <c r="C73">
         <v>0</v>

</xml_diff>